<commit_message>
Update template for files
</commit_message>
<xml_diff>
--- a/templates/Account Files.xlsx
+++ b/templates/Account Files.xlsx
@@ -38,18 +38,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>A description for the file</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Account ID</t>
   </si>
   <si>
     <t>File</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
@@ -91,7 +106,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +117,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,12 +160,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,6 +303,18 @@
           </a:r>
           <a:endParaRPr/>
         </a:p>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" spc="-1">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Grey columns are required, blue columns are optional.</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -317,16 +354,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,6 +374,9 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>